<commit_message>
Atnaujintas TS test Summary
Atnaujintas TS test Summary
</commit_message>
<xml_diff>
--- a/docs/Test Summary Report 2023-12-10_TS.xlsx
+++ b/docs/Test Summary Report 2023-12-10_TS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\Desktop\testCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220F142B-9379-4299-B5C7-416FECB2FA78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACCDB35-0520-49B4-85ED-642C86A3A906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -128,10 +128,10 @@
     <t>Windows11 home Version 23H2</t>
   </si>
   <si>
-    <t>Pass</t>
-  </si>
-  <si>
     <t>Pagrindines klaidos buvo: neatidus spalvu kodu parinkimas pagal duota uzduoti. Teksto srifto, dydzio , formatavimo nevienodumas.</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -496,8 +496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,7 +659,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -667,7 +667,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">

</xml_diff>